<commit_message>
Adjust SSFA_2 and SSFA_3 with v8.2 datasets
- remove checksums
- Zoomed plots for Smfc with values <= 10
- Adjust box width (automatically)
</commit_message>
<xml_diff>
--- a/R_analysis/summary_stats/SSFA_summary_stats.xlsx
+++ b/R_analysis/summary_stats/SSFA_summary_stats.xlsx
@@ -161,13 +161,13 @@
     <t xml:space="preserve">ConfoMap</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry Bamboo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Grass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Lucerne</t>
+    <t xml:space="preserve">Dry bamboo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry grass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry lucerne</t>
   </si>
   <si>
     <t xml:space="preserve">Toothfrax</t>
@@ -176,37 +176,37 @@
     <t xml:space="preserve">Lithics</t>
   </si>
   <si>
+    <t xml:space="preserve">Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RubDirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BrushNoDirt</t>
+  </si>
+  <si>
     <t xml:space="preserve">BrushDirt</t>
   </si>
   <si>
-    <t xml:space="preserve">Before</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BrushNoDirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RubDirt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sheeps</t>
   </si>
   <si>
     <t xml:space="preserve">Clover</t>
   </si>
   <si>
-    <t xml:space="preserve">Clover+Dust</t>
+    <t xml:space="preserve">Clover+dust</t>
   </si>
   <si>
     <t xml:space="preserve">Grass</t>
   </si>
   <si>
-    <t xml:space="preserve">Grass+Dust</t>
+    <t xml:space="preserve">Grass+dust</t>
   </si>
 </sst>
 </file>
@@ -697,127 +697,127 @@
         <v>24</v>
       </c>
       <c r="G2" t="n">
-        <v>0.002936327</v>
+        <v>0.003078460776</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00730538</v>
+        <v>0.007515140223</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00510848545833333</v>
+        <v>0.005314470743</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0052226305</v>
+        <v>0.0054224162775</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00106278043307351</v>
+        <v>0.00108723408632173</v>
       </c>
       <c r="L2" t="n">
         <v>24</v>
       </c>
       <c r="M2" t="n">
-        <v>0.997718162</v>
+        <v>0.9976183271</v>
       </c>
       <c r="N2" t="n">
-        <v>0.999553351</v>
+        <v>0.9988392089</v>
       </c>
       <c r="O2" t="n">
-        <v>0.99855178875</v>
+        <v>0.9982640154</v>
       </c>
       <c r="P2" t="n">
-        <v>0.998582844</v>
+        <v>0.9983230352</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.000513880172336544</v>
+        <v>0.000340004994482393</v>
       </c>
       <c r="R2" t="n">
         <v>24</v>
       </c>
       <c r="S2" t="n">
-        <v>10.53507997</v>
+        <v>6.752552626</v>
       </c>
       <c r="T2" t="n">
-        <v>32.31299832</v>
+        <v>28.0022206</v>
       </c>
       <c r="U2" t="n">
-        <v>17.4191368454167</v>
+        <v>13.43554427775</v>
       </c>
       <c r="V2" t="n">
-        <v>16.346221295</v>
+        <v>11.96508713</v>
       </c>
       <c r="W2" t="n">
-        <v>6.10186803478364</v>
+        <v>5.71466560156411</v>
       </c>
       <c r="X2" t="n">
         <v>24</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.229333441</v>
+        <v>0.4014873099</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.52681366</v>
+        <v>0.7378979554</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.356710740625</v>
+        <v>0.538971141304167</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.3582229325</v>
+        <v>0.57547933905</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0606203856381962</v>
+        <v>0.0958007122491773</v>
       </c>
       <c r="AD2" t="n">
         <v>24</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.124791542</v>
+        <v>0.118869778</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.2886548</v>
+        <v>0.3095299721</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.208107762333333</v>
+        <v>0.2173132965375</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.2097812805</v>
+        <v>0.21239244035</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0483692791820207</v>
+        <v>0.0502711079429104</v>
       </c>
       <c r="AJ2" t="n">
         <v>24</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.251486818</v>
+        <v>0.2909851406</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.450188396</v>
+        <v>0.4859585013</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.35963789125</v>
+        <v>0.3829782341375</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.3692192075</v>
+        <v>0.387370277</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.0489201396343252</v>
+        <v>0.0541701761768203</v>
       </c>
       <c r="AP2" t="n">
         <v>24</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.018769595</v>
+        <v>0.01882726172</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.020693929</v>
+        <v>0.02078594416</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.019763261625</v>
+        <v>0.0198514564495833</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.019810148</v>
+        <v>0.019900900555</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.000473654554872312</v>
+        <v>0.000484981832389577</v>
       </c>
     </row>
     <row r="3">
@@ -836,127 +836,127 @@
         <v>22</v>
       </c>
       <c r="G3" t="n">
-        <v>0.000321969</v>
+        <v>0.0003473793101</v>
       </c>
       <c r="H3" t="n">
-        <v>0.005335126</v>
+        <v>0.005525790493</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00185800540909091</v>
+        <v>0.00194611353211364</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001598577</v>
+        <v>0.0016550119995</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00111606269415104</v>
+        <v>0.00114842705461904</v>
       </c>
       <c r="L3" t="n">
         <v>22</v>
       </c>
       <c r="M3" t="n">
-        <v>0.998192145</v>
+        <v>0.9973204701</v>
       </c>
       <c r="N3" t="n">
-        <v>0.999138808</v>
+        <v>0.9989523375</v>
       </c>
       <c r="O3" t="n">
-        <v>0.998661824863636</v>
+        <v>0.998213250486364</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9987061505</v>
+        <v>0.9982578275</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.000279587413487789</v>
+        <v>0.00042256013705016</v>
       </c>
       <c r="R3" t="n">
         <v>22</v>
       </c>
       <c r="S3" t="n">
-        <v>10.13463639</v>
+        <v>5.934820597</v>
       </c>
       <c r="T3" t="n">
-        <v>24.01503378</v>
+        <v>18.89177552</v>
       </c>
       <c r="U3" t="n">
-        <v>14.7793717854545</v>
+        <v>11.0567587424545</v>
       </c>
       <c r="V3" t="n">
-        <v>13.65801498</v>
+        <v>9.5129279065</v>
       </c>
       <c r="W3" t="n">
-        <v>3.84570118224138</v>
+        <v>3.62363581072559</v>
       </c>
       <c r="X3" t="n">
         <v>22</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.160572744</v>
+        <v>0.2308749621</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.62958563</v>
+        <v>0.6981790427</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.378702026181818</v>
+        <v>0.508097090059091</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.380147943</v>
+        <v>0.5445029507</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.107190804825888</v>
+        <v>0.127415519070416</v>
       </c>
       <c r="AD3" t="n">
         <v>22</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.151634155</v>
+        <v>0.1612149107</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.561422278</v>
+        <v>0.496191823</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.311236265454545</v>
+        <v>0.301399650272727</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.288945062</v>
+        <v>0.2838729157</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.139312190675551</v>
+        <v>0.118848407291162</v>
       </c>
       <c r="AJ3" t="n">
         <v>22</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.277592374</v>
+        <v>0.267574094</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.613802752</v>
+        <v>0.599353621</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.439830230227273</v>
+        <v>0.432996452163636</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.426158205</v>
+        <v>0.43990007015</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.0965530533179395</v>
+        <v>0.0804087259588066</v>
       </c>
       <c r="AP3" t="n">
         <v>22</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.017288718</v>
+        <v>0.01727077648</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.01979391</v>
+        <v>0.01987551916</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.0180153917727273</v>
+        <v>0.0180341163545455</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.018023439</v>
+        <v>0.01805577033</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.000626142891182191</v>
+        <v>0.000653364702916592</v>
       </c>
     </row>
     <row r="4">
@@ -975,127 +975,127 @@
         <v>24</v>
       </c>
       <c r="G4" t="n">
-        <v>0.001195386</v>
+        <v>0.001256082569</v>
       </c>
       <c r="H4" t="n">
-        <v>0.004348138</v>
+        <v>0.004547933282</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00257509041666667</v>
+        <v>0.00270259997025</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0025059445</v>
+        <v>0.00263209676</v>
       </c>
       <c r="K4" t="n">
-        <v>0.000891140034568516</v>
+        <v>0.000921483704289703</v>
       </c>
       <c r="L4" t="n">
         <v>24</v>
       </c>
       <c r="M4" t="n">
-        <v>0.997532386</v>
+        <v>0.9979155975</v>
       </c>
       <c r="N4" t="n">
-        <v>0.999112342</v>
+        <v>0.9989192509</v>
       </c>
       <c r="O4" t="n">
-        <v>0.998624484708333</v>
+        <v>0.998388261841667</v>
       </c>
       <c r="P4" t="n">
-        <v>0.998811998</v>
+        <v>0.9984053993</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.000448563392089295</v>
+        <v>0.000254357795499881</v>
       </c>
       <c r="R4" t="n">
         <v>24</v>
       </c>
       <c r="S4" t="n">
-        <v>8.951343639</v>
+        <v>5.524081785</v>
       </c>
       <c r="T4" t="n">
-        <v>19.57223708</v>
+        <v>15.72230321</v>
       </c>
       <c r="U4" t="n">
-        <v>13.2283176405417</v>
+        <v>9.887051880875</v>
       </c>
       <c r="V4" t="n">
-        <v>13.22726666</v>
+        <v>10.0148848395</v>
       </c>
       <c r="W4" t="n">
-        <v>2.70832860219084</v>
+        <v>2.39533136490601</v>
       </c>
       <c r="X4" t="n">
         <v>24</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.216106648</v>
+        <v>0.3400817502</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.496429712</v>
+        <v>0.6605980842</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.37543850075</v>
+        <v>0.526657080604167</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.380147943</v>
+        <v>0.57547933905</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.0842742818271462</v>
+        <v>0.102352527029535</v>
       </c>
       <c r="AD4" t="n">
         <v>24</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.120905484</v>
+        <v>0.0982992664</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.428999312</v>
+        <v>0.4021779541</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.238532968333333</v>
+        <v>0.242458666866667</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.205296485</v>
+        <v>0.21022775695</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.091333793822781</v>
+        <v>0.0910770512821215</v>
       </c>
       <c r="AJ4" t="n">
         <v>24</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.309204915</v>
+        <v>0.3176914814</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.855690281</v>
+        <v>0.9249893402</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.448902190166667</v>
+        <v>0.449223858854167</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.409760765</v>
+        <v>0.42077119535</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.121879119124477</v>
+        <v>0.131144244707378</v>
       </c>
       <c r="AP4" t="n">
         <v>24</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.018068187</v>
+        <v>0.01811085623</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.019249182</v>
+        <v>0.01930272211</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.018542003125</v>
+        <v>0.0185934354620833</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.018538167</v>
+        <v>0.018586015155</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.00034907076303166</v>
+        <v>0.000361319409664501</v>
       </c>
     </row>
     <row r="5">
@@ -1518,130 +1518,130 @@
         <v>55</v>
       </c>
       <c r="F8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001086565</v>
+        <v>0.0002936432628</v>
       </c>
       <c r="H8" t="n">
-        <v>0.002873698</v>
+        <v>0.000919971656</v>
       </c>
       <c r="I8" t="n">
-        <v>0.00211750475</v>
+        <v>0.0006669765454</v>
       </c>
       <c r="J8" t="n">
-        <v>0.002254878</v>
+        <v>0.0007873147174</v>
       </c>
       <c r="K8" t="n">
-        <v>0.000878920044212356</v>
+        <v>0.000330049648935353</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>0.998181677</v>
+        <v>0.9687007925</v>
       </c>
       <c r="N8" t="n">
-        <v>0.999493818</v>
+        <v>0.9975038456</v>
       </c>
       <c r="O8" t="n">
-        <v>0.99873090575</v>
+        <v>0.987763637433333</v>
       </c>
       <c r="P8" t="n">
-        <v>0.998624064</v>
+        <v>0.9970862742</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.000606394009021305</v>
+        <v>0.0165102281687068</v>
       </c>
       <c r="R8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S8" t="n">
-        <v>27.83710297</v>
+        <v>32.93456721</v>
       </c>
       <c r="T8" t="n">
-        <v>42.47753596</v>
+        <v>48.65456508</v>
       </c>
       <c r="U8" t="n">
-        <v>34.3437969725</v>
+        <v>40.8371878566667</v>
       </c>
       <c r="V8" t="n">
-        <v>33.53027448</v>
+        <v>40.92243128</v>
       </c>
       <c r="W8" t="n">
-        <v>7.45671267688221</v>
+        <v>7.86034560875776</v>
       </c>
       <c r="X8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z8" t="n">
-        <v>29.75060383</v>
+        <v>0.3720763218</v>
       </c>
       <c r="AA8" t="n">
-        <v>7.5113562145</v>
+        <v>0.252044146033333</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.098273676</v>
+        <v>0.2352792781</v>
       </c>
       <c r="AC8" t="n">
-        <v>14.826165077</v>
+        <v>0.11258978835411</v>
       </c>
       <c r="AD8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.115494724</v>
+        <v>0.1648586724</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.299872426</v>
+        <v>0.2825431635</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.2037951915</v>
+        <v>0.2398719499</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.199906808</v>
+        <v>0.2722140138</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.0878209368088846</v>
+        <v>0.0651683718098761</v>
       </c>
       <c r="AJ8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.181728511</v>
+        <v>0.2494563427</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.52126036</v>
+        <v>0.4869355776</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.3256512825</v>
+        <v>0.377840660333333</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.2998081295</v>
+        <v>0.3971300607</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.167094573812765</v>
+        <v>0.119908954949376</v>
       </c>
       <c r="AP8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.017208908</v>
+        <v>0.01735927631</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.018695971</v>
+        <v>0.01802049863</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.01791702025</v>
+        <v>0.01767043174</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.017881601</v>
+        <v>0.01763152028</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.000736390314108569</v>
+        <v>0.000332324111984135</v>
       </c>
     </row>
     <row r="9">
@@ -1659,130 +1659,130 @@
         <v>56</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0000187</v>
+        <v>0.0008689380972</v>
       </c>
       <c r="H9" t="n">
-        <v>0.004908073</v>
+        <v>0.002119448847</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00184288775</v>
+        <v>0.00129481443283333</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001222389</v>
+        <v>0.0008960563543</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00212813510583177</v>
+        <v>0.000714283058554546</v>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
-        <v>0.998017587</v>
+        <v>0.9668825284</v>
       </c>
       <c r="N9" t="n">
-        <v>0.998885923</v>
+        <v>0.9979706128</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9985067965</v>
+        <v>0.980052246933333</v>
       </c>
       <c r="P9" t="n">
-        <v>0.998561838</v>
+        <v>0.9753035996</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.000429944335082661</v>
+        <v>0.0160788521523665</v>
       </c>
       <c r="R9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" t="n">
-        <v>41.7451596</v>
+        <v>36.60732582</v>
       </c>
       <c r="T9" t="n">
-        <v>52.15774541</v>
+        <v>57.90574331</v>
       </c>
       <c r="U9" t="n">
-        <v>45.6059140475</v>
+        <v>47.32836902</v>
       </c>
       <c r="V9" t="n">
-        <v>44.26037559</v>
+        <v>47.47203793</v>
       </c>
       <c r="W9" t="n">
-        <v>4.61315373581192</v>
+        <v>10.6499355613712</v>
       </c>
       <c r="X9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.090676075</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z9" t="n">
-        <v>6.990287164</v>
+        <v>106.0624695</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.90813337725</v>
+        <v>35.4821752054333</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.275785135</v>
+        <v>0.2352792781</v>
       </c>
       <c r="AC9" t="n">
-        <v>3.39232370516067</v>
+        <v>61.1243431678309</v>
       </c>
       <c r="AD9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.098946404</v>
+        <v>0.1969198415</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.477906688</v>
+        <v>0.9607836648</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2669586355</v>
+        <v>0.513918029566667</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.245490725</v>
+        <v>0.3840505824</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.193433530110394</v>
+        <v>0.398147146808581</v>
       </c>
       <c r="AJ9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.15843918</v>
+        <v>0.2576204095</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.693555248</v>
+        <v>1.427259549</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.4227858955</v>
+        <v>0.740123661633333</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.419574577</v>
+        <v>0.5354910264</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.304814366878102</v>
+        <v>0.611080858573134</v>
       </c>
       <c r="AP9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.017082766</v>
+        <v>0.0172858608</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.019741438</v>
+        <v>0.01740630779</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.0181229215</v>
+        <v>0.01733728303</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.017833741</v>
+        <v>0.0173196805</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.00114430990702854</v>
+        <v>0.0000621229116092895</v>
       </c>
     </row>
     <row r="10">
@@ -1803,127 +1803,127 @@
         <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000824688</v>
+        <v>0.0004941669981</v>
       </c>
       <c r="H10" t="n">
-        <v>0.002451287</v>
+        <v>0.001649800079</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0017083615</v>
+        <v>0.001071093918025</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0017787355</v>
+        <v>0.0010702042975</v>
       </c>
       <c r="K10" t="n">
-        <v>0.000802685988087704</v>
+        <v>0.000472144493867255</v>
       </c>
       <c r="L10" t="n">
         <v>4</v>
       </c>
       <c r="M10" t="n">
-        <v>0.995932428</v>
+        <v>0.9541553811</v>
       </c>
       <c r="N10" t="n">
-        <v>0.998403963</v>
+        <v>0.9982468999</v>
       </c>
       <c r="O10" t="n">
-        <v>0.997691151</v>
+        <v>0.97595091575</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9982141065</v>
+        <v>0.975700691</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.00117786460450171</v>
+        <v>0.0247948934709663</v>
       </c>
       <c r="R10" t="n">
         <v>4</v>
       </c>
       <c r="S10" t="n">
-        <v>35.85415864</v>
+        <v>32.634796</v>
       </c>
       <c r="T10" t="n">
-        <v>60.77933788</v>
+        <v>60.59286224</v>
       </c>
       <c r="U10" t="n">
-        <v>44.33367301</v>
+        <v>45.00906551</v>
       </c>
       <c r="V10" t="n">
-        <v>40.35059776</v>
+        <v>43.4043019</v>
       </c>
       <c r="W10" t="n">
-        <v>11.3542337763208</v>
+        <v>13.1330947413026</v>
       </c>
       <c r="X10" t="n">
         <v>4</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.125103846</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z10" t="n">
-        <v>78.13212386</v>
+        <v>31.24396363</v>
       </c>
       <c r="AA10" t="n">
-        <v>23.835760502</v>
+        <v>12.8245925866</v>
       </c>
       <c r="AB10" t="n">
-        <v>8.542907151</v>
+        <v>9.9528149391</v>
       </c>
       <c r="AC10" t="n">
-        <v>37.0540926496488</v>
+        <v>15.369689591346</v>
       </c>
       <c r="AD10" t="n">
         <v>4</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.120464395</v>
+        <v>0.1001065453</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.752312797</v>
+        <v>0.6153930042</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.36384240925</v>
+        <v>0.2733492024</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.2912962225</v>
+        <v>0.18894863005</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.301891301135017</v>
+        <v>0.239921159504009</v>
       </c>
       <c r="AJ10" t="n">
         <v>4</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.130787072</v>
+        <v>0.1573114157</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.900819911</v>
+        <v>1.171104075</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.45478912325</v>
+        <v>0.52749616125</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.393774755</v>
+        <v>0.39078457715</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.371351909719787</v>
+        <v>0.471701735451469</v>
       </c>
       <c r="AP10" t="n">
         <v>4</v>
       </c>
       <c r="AQ10" t="n">
-        <v>0.017451291</v>
+        <v>0.01702138679</v>
       </c>
       <c r="AR10" t="n">
-        <v>0.018228484</v>
+        <v>0.01775102777</v>
       </c>
       <c r="AS10" t="n">
-        <v>0.0178304775</v>
+        <v>0.01740949782</v>
       </c>
       <c r="AT10" t="n">
-        <v>0.0178210675</v>
+        <v>0.01743278836</v>
       </c>
       <c r="AU10" t="n">
-        <v>0.000421519686597988</v>
+        <v>0.000302699305814026</v>
       </c>
     </row>
     <row r="11">
@@ -1944,127 +1944,127 @@
         <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000479482</v>
+        <v>0.001018217068</v>
       </c>
       <c r="H11" t="n">
-        <v>0.002453128</v>
+        <v>0.003526645148</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00152806525</v>
+        <v>0.00179330141825</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0015898255</v>
+        <v>0.0013141717285</v>
       </c>
       <c r="K11" t="n">
-        <v>0.000818225140390009</v>
+        <v>0.00117814688647876</v>
       </c>
       <c r="L11" t="n">
         <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>0.998011514</v>
+        <v>0.9781051126</v>
       </c>
       <c r="N11" t="n">
-        <v>0.999325468</v>
+        <v>0.9994579584</v>
       </c>
       <c r="O11" t="n">
-        <v>0.99852302675</v>
+        <v>0.993293344925</v>
       </c>
       <c r="P11" t="n">
-        <v>0.9983775625</v>
+        <v>0.99780515435</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.000599856798239583</v>
+        <v>0.0101668558796136</v>
       </c>
       <c r="R11" t="n">
         <v>4</v>
       </c>
       <c r="S11" t="n">
-        <v>31.93174348</v>
+        <v>20.50910277</v>
       </c>
       <c r="T11" t="n">
-        <v>56.10034375</v>
+        <v>57.75443619</v>
       </c>
       <c r="U11" t="n">
-        <v>44.8078730925</v>
+        <v>40.745907875</v>
       </c>
       <c r="V11" t="n">
-        <v>45.59970257</v>
+        <v>42.36004627</v>
       </c>
       <c r="W11" t="n">
-        <v>9.94759191751666</v>
+        <v>16.1614708118047</v>
       </c>
       <c r="X11" t="n">
         <v>4</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.106507867</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z11" t="n">
-        <v>11.32822691</v>
+        <v>24.8451685</v>
       </c>
       <c r="AA11" t="n">
-        <v>3.410260009</v>
+        <v>11.9193264453</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.1031526295</v>
+        <v>11.3416802215</v>
       </c>
       <c r="AC11" t="n">
-        <v>5.36052395180043</v>
+        <v>12.2191222860787</v>
       </c>
       <c r="AD11" t="n">
         <v>4</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.092286484</v>
+        <v>0.1166349597</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.45591596</v>
+        <v>0.5858252931</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.2480467705</v>
+        <v>0.296347003675</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.221992319</v>
+        <v>0.24146388095</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.169687577847732</v>
+        <v>0.209534240034722</v>
       </c>
       <c r="AJ11" t="n">
         <v>4</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.132139707</v>
+        <v>0.2612446632</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.808554753</v>
+        <v>0.9463857716</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.40372541775</v>
+        <v>0.4986485467</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.3371036055</v>
+        <v>0.393481876</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.312560671658728</v>
+        <v>0.321219996575637</v>
       </c>
       <c r="AP11" t="n">
         <v>4</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0.01764173</v>
+        <v>0.01707299971</v>
       </c>
       <c r="AR11" t="n">
-        <v>0.018445122</v>
+        <v>0.01789620905</v>
       </c>
       <c r="AS11" t="n">
-        <v>0.0180651495</v>
+        <v>0.017432186015</v>
       </c>
       <c r="AT11" t="n">
-        <v>0.018086873</v>
+        <v>0.01737976765</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.000434039042158268</v>
+        <v>0.000359388551604808</v>
       </c>
     </row>
     <row r="12">
@@ -2082,130 +2082,130 @@
         <v>55</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000343256</v>
+        <v>0.0007937613179</v>
       </c>
       <c r="H12" t="n">
-        <v>0.000868187</v>
+        <v>0.002608418627</v>
       </c>
       <c r="I12" t="n">
-        <v>0.000659720666666667</v>
+        <v>0.001781266699475</v>
       </c>
       <c r="J12" t="n">
-        <v>0.000767719</v>
+        <v>0.0018614434265</v>
       </c>
       <c r="K12" t="n">
-        <v>0.000278632138656569</v>
+        <v>0.000854800136114038</v>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
-        <v>0.99800771</v>
+        <v>0.9942276257</v>
       </c>
       <c r="N12" t="n">
-        <v>0.998742978</v>
+        <v>0.9969253405</v>
       </c>
       <c r="O12" t="n">
-        <v>0.998258422</v>
+        <v>0.9959657545</v>
       </c>
       <c r="P12" t="n">
-        <v>0.998024578</v>
+        <v>0.9963550259</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.000419722551464661</v>
+        <v>0.0011952272026332</v>
       </c>
       <c r="R12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S12" t="n">
-        <v>42.18953537</v>
+        <v>33.3489681</v>
       </c>
       <c r="T12" t="n">
-        <v>52.56948935</v>
+        <v>64.88962328</v>
       </c>
       <c r="U12" t="n">
-        <v>46.51074729</v>
+        <v>42.9135262725</v>
       </c>
       <c r="V12" t="n">
-        <v>44.77321715</v>
+        <v>36.707756855</v>
       </c>
       <c r="W12" t="n">
-        <v>5.40371348216074</v>
+        <v>14.760116118204</v>
       </c>
       <c r="X12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.418251945</v>
+        <v>78.13809733</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.265413492333333</v>
+        <v>28.7092101141</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.279714856</v>
+        <v>18.2749831441</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.160467815807731</v>
+        <v>37.120426251685</v>
       </c>
       <c r="AD12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.154945531</v>
+        <v>0.1078059316</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.310355073</v>
+        <v>0.7440534086</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.242566174333333</v>
+        <v>0.37377898425</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.262397919</v>
+        <v>0.3216282984</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.0795801797469404</v>
+        <v>0.306289508719417</v>
       </c>
       <c r="AJ12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.196330737</v>
+        <v>0.1681378255</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.445268964</v>
+        <v>0.8756408545</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.352791647666667</v>
+        <v>0.494786954175</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.416775242</v>
+        <v>0.46768456835</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.136246047551242</v>
+        <v>0.34712791915946</v>
       </c>
       <c r="AP12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ12" t="n">
-        <v>0.017367301</v>
+        <v>0.01746284442</v>
       </c>
       <c r="AR12" t="n">
-        <v>0.018009401</v>
+        <v>0.01830269105</v>
       </c>
       <c r="AS12" t="n">
-        <v>0.0176788903333333</v>
+        <v>0.0178783006425</v>
       </c>
       <c r="AT12" t="n">
-        <v>0.017659969</v>
+        <v>0.01787383355</v>
       </c>
       <c r="AU12" t="n">
-        <v>0.000321467906860597</v>
+        <v>0.000466533308937529</v>
       </c>
     </row>
     <row r="13">
@@ -2223,130 +2223,130 @@
         <v>56</v>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000776606</v>
+        <v>0.000491684713</v>
       </c>
       <c r="H13" t="n">
-        <v>0.001727267</v>
+        <v>0.002461238008</v>
       </c>
       <c r="I13" t="n">
-        <v>0.00111072933333333</v>
+        <v>0.00159145502625</v>
       </c>
       <c r="J13" t="n">
-        <v>0.000828315</v>
+        <v>0.001706448692</v>
       </c>
       <c r="K13" t="n">
-        <v>0.000534562883096398</v>
+        <v>0.000855713850189721</v>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>0.983654412</v>
+        <v>0.9744148084</v>
       </c>
       <c r="N13" t="n">
-        <v>0.998398191</v>
+        <v>0.9991265816</v>
       </c>
       <c r="O13" t="n">
-        <v>0.993479191666667</v>
+        <v>0.986794324</v>
       </c>
       <c r="P13" t="n">
-        <v>0.998384972</v>
+        <v>0.986817953</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.00850851134508265</v>
+        <v>0.0134210928431656</v>
       </c>
       <c r="R13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S13" t="n">
-        <v>46.23666979</v>
+        <v>32.36781714</v>
       </c>
       <c r="T13" t="n">
-        <v>53.74611704</v>
+        <v>54.82280245</v>
       </c>
       <c r="U13" t="n">
-        <v>50.2841795566667</v>
+        <v>40.1467427725</v>
       </c>
       <c r="V13" t="n">
-        <v>50.86975184</v>
+        <v>36.69817575</v>
       </c>
       <c r="W13" t="n">
-        <v>3.78881520721047</v>
+        <v>10.0059238000465</v>
       </c>
       <c r="X13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z13" t="n">
-        <v>241.0196487</v>
+        <v>19.75685304</v>
       </c>
       <c r="AA13" t="n">
-        <v>80.4821582243333</v>
+        <v>9.9528149391</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.328552297</v>
+        <v>9.9528149391</v>
       </c>
       <c r="AC13" t="n">
-        <v>139.029592688857</v>
+        <v>11.3207280733999</v>
       </c>
       <c r="AD13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.176976089</v>
+        <v>0.100009045</v>
       </c>
       <c r="AF13" t="n">
-        <v>1.292871138</v>
+        <v>0.4693025626</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.602116383666667</v>
+        <v>0.252128765625</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.336501924</v>
+        <v>0.21960172745</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.603505361188854</v>
+        <v>0.165832740268222</v>
       </c>
       <c r="AJ13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK13" t="n">
-        <v>0.214938239</v>
+        <v>0.1524915323</v>
       </c>
       <c r="AL13" t="n">
-        <v>1.692403539</v>
+        <v>0.8144845581</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.797734089666667</v>
+        <v>0.414176555475</v>
       </c>
       <c r="AN13" t="n">
-        <v>0.485860491</v>
+        <v>0.34486506575</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.786558824459427</v>
+        <v>0.298391572933595</v>
       </c>
       <c r="AP13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ13" t="n">
-        <v>0.017335313</v>
+        <v>0.01762566378</v>
       </c>
       <c r="AR13" t="n">
-        <v>0.017474255</v>
+        <v>0.01855063605</v>
       </c>
       <c r="AS13" t="n">
-        <v>0.0173903616666667</v>
+        <v>0.0181063534575</v>
       </c>
       <c r="AT13" t="n">
-        <v>0.017361517</v>
+        <v>0.018124557</v>
       </c>
       <c r="AU13" t="n">
-        <v>0.0000738256793895819</v>
+        <v>0.000490304077008518</v>
       </c>
     </row>
     <row r="14">
@@ -2367,127 +2367,127 @@
         <v>4</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000396267</v>
+        <v>0.00112382419</v>
       </c>
       <c r="H14" t="n">
-        <v>0.001481818</v>
+        <v>0.003139539945</v>
       </c>
       <c r="I14" t="n">
-        <v>0.00099238725</v>
+        <v>0.0021512726665</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001045732</v>
+        <v>0.0021708632655</v>
       </c>
       <c r="K14" t="n">
-        <v>0.000447567343614623</v>
+        <v>0.000892758950261954</v>
       </c>
       <c r="L14" t="n">
         <v>4</v>
       </c>
       <c r="M14" t="n">
-        <v>0.998117027</v>
+        <v>0.9645403369</v>
       </c>
       <c r="N14" t="n">
-        <v>0.999052642</v>
+        <v>0.9981351597</v>
       </c>
       <c r="O14" t="n">
-        <v>0.99858865125</v>
+        <v>0.981435700775</v>
       </c>
       <c r="P14" t="n">
-        <v>0.998592468</v>
+        <v>0.98153365325</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.000494354956919528</v>
+        <v>0.0192789028605277</v>
       </c>
       <c r="R14" t="n">
         <v>4</v>
       </c>
       <c r="S14" t="n">
-        <v>42.47218426</v>
+        <v>27.60120501</v>
       </c>
       <c r="T14" t="n">
-        <v>58.93295166</v>
+        <v>33.25588838</v>
       </c>
       <c r="U14" t="n">
-        <v>49.104086955</v>
+        <v>29.9652554875</v>
       </c>
       <c r="V14" t="n">
-        <v>47.50560595</v>
+        <v>29.50196428</v>
       </c>
       <c r="W14" t="n">
-        <v>7.13200087721157</v>
+        <v>2.45821033640548</v>
       </c>
       <c r="X14" t="n">
         <v>4</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.090676075</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z14" t="n">
-        <v>14.4210008</v>
+        <v>28.9461893</v>
       </c>
       <c r="AA14" t="n">
-        <v>6.72183778775</v>
+        <v>12.2501490041</v>
       </c>
       <c r="AB14" t="n">
-        <v>6.187837138</v>
+        <v>9.9528149391</v>
       </c>
       <c r="AC14" t="n">
-        <v>7.70249518994024</v>
+        <v>14.4682961867221</v>
       </c>
       <c r="AD14" t="n">
         <v>4</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.091605465</v>
+        <v>0.1320614168</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.593606267</v>
+        <v>0.4189861196</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.258043442</v>
+        <v>0.27820914495</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.173481018</v>
+        <v>0.2808945217</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.233185997002481</v>
+        <v>0.159663483071599</v>
       </c>
       <c r="AJ14" t="n">
         <v>4</v>
       </c>
       <c r="AK14" t="n">
-        <v>0.12475774</v>
+        <v>0.2277337819</v>
       </c>
       <c r="AL14" t="n">
-        <v>1.173067077</v>
+        <v>0.8136697615</v>
       </c>
       <c r="AM14" t="n">
-        <v>0.5040660485</v>
+        <v>0.48365606455</v>
       </c>
       <c r="AN14" t="n">
-        <v>0.3592196885</v>
+        <v>0.4466103574</v>
       </c>
       <c r="AO14" t="n">
-        <v>0.488403527809425</v>
+        <v>0.29514389195903</v>
       </c>
       <c r="AP14" t="n">
         <v>4</v>
       </c>
       <c r="AQ14" t="n">
-        <v>0.017130761</v>
+        <v>0.01719386889</v>
       </c>
       <c r="AR14" t="n">
-        <v>0.017737721</v>
+        <v>0.01881955794</v>
       </c>
       <c r="AS14" t="n">
-        <v>0.0174343705</v>
+        <v>0.0179589111175</v>
       </c>
       <c r="AT14" t="n">
-        <v>0.0174345</v>
+        <v>0.01791110882</v>
       </c>
       <c r="AU14" t="n">
-        <v>0.000251659391750702</v>
+        <v>0.00079849133580769</v>
       </c>
     </row>
     <row r="15">
@@ -2508,127 +2508,127 @@
         <v>4</v>
       </c>
       <c r="G15" t="n">
-        <v>0.000845547</v>
+        <v>0.00003663171778</v>
       </c>
       <c r="H15" t="n">
-        <v>0.003466463</v>
+        <v>0.00520758282</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00166693075</v>
+        <v>0.001962484484695</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0011778565</v>
+        <v>0.0013028617005</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00121275628867534</v>
+        <v>0.00225006844187079</v>
       </c>
       <c r="L15" t="n">
         <v>4</v>
       </c>
       <c r="M15" t="n">
-        <v>0.99807401</v>
+        <v>0.9622675292</v>
       </c>
       <c r="N15" t="n">
-        <v>0.998833174</v>
+        <v>0.9983590376</v>
       </c>
       <c r="O15" t="n">
-        <v>0.9985300395</v>
+        <v>0.980625522875</v>
       </c>
       <c r="P15" t="n">
-        <v>0.998606487</v>
+        <v>0.98093776235</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.000342740422132681</v>
+        <v>0.020166478365834</v>
       </c>
       <c r="R15" t="n">
         <v>4</v>
       </c>
       <c r="S15" t="n">
-        <v>20.28081709</v>
+        <v>32.21166602</v>
       </c>
       <c r="T15" t="n">
-        <v>53.72619817</v>
+        <v>51.36728127</v>
       </c>
       <c r="U15" t="n">
-        <v>41.3044528725</v>
+        <v>40.7357046975</v>
       </c>
       <c r="V15" t="n">
-        <v>45.605398115</v>
+        <v>39.68193575</v>
       </c>
       <c r="W15" t="n">
-        <v>14.6146526315626</v>
+        <v>8.66611339636906</v>
       </c>
       <c r="X15" t="n">
         <v>4</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.125103846</v>
+        <v>0.1487768382</v>
       </c>
       <c r="Z15" t="n">
-        <v>16.93886767</v>
+        <v>15.7106297</v>
       </c>
       <c r="AA15" t="n">
-        <v>5.4778693455</v>
+        <v>4.060865663625</v>
       </c>
       <c r="AB15" t="n">
-        <v>2.423752933</v>
+        <v>0.19202805815</v>
       </c>
       <c r="AC15" t="n">
-        <v>7.93299410223379</v>
+        <v>7.76661640725571</v>
       </c>
       <c r="AD15" t="n">
         <v>4</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.090791297</v>
+        <v>0.112306445</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.603800166</v>
+        <v>0.414137293</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.2630387355</v>
+        <v>0.255463651325</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.1787817395</v>
+        <v>0.24770543365</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.232851547777254</v>
+        <v>0.162289322930355</v>
       </c>
       <c r="AJ15" t="n">
         <v>4</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.216962845</v>
+        <v>0.2011162269</v>
       </c>
       <c r="AL15" t="n">
-        <v>0.969789081</v>
+        <v>0.7504292451</v>
       </c>
       <c r="AM15" t="n">
-        <v>0.47398638075</v>
+        <v>0.4550364292</v>
       </c>
       <c r="AN15" t="n">
-        <v>0.3545967985</v>
+        <v>0.4343001224</v>
       </c>
       <c r="AO15" t="n">
-        <v>0.354062089382092</v>
+        <v>0.294527608294164</v>
       </c>
       <c r="AP15" t="n">
         <v>4</v>
       </c>
       <c r="AQ15" t="n">
-        <v>0.017165356</v>
+        <v>0.01706059375</v>
       </c>
       <c r="AR15" t="n">
-        <v>0.01786269</v>
+        <v>0.01989473552</v>
       </c>
       <c r="AS15" t="n">
-        <v>0.01746874325</v>
+        <v>0.018172740075</v>
       </c>
       <c r="AT15" t="n">
-        <v>0.0174234635</v>
+        <v>0.017867815515</v>
       </c>
       <c r="AU15" t="n">
-        <v>0.000299195631063663</v>
+        <v>0.00122131529699802</v>
       </c>
     </row>
     <row r="16">
@@ -2646,112 +2646,112 @@
         <v>55</v>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00133</v>
+        <v>0.000149</v>
       </c>
       <c r="H16" t="n">
-        <v>0.002509</v>
+        <v>0.000899</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0016735</v>
+        <v>0.000574666666666667</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0014275</v>
+        <v>0.000676</v>
       </c>
       <c r="K16" t="n">
-        <v>0.000562193620265</v>
+        <v>0.000385131579247059</v>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
-        <v>0.996841</v>
+        <v>0.999197</v>
       </c>
       <c r="N16" t="n">
-        <v>0.99946</v>
+        <v>0.999765</v>
       </c>
       <c r="O16" t="n">
-        <v>0.99853325</v>
+        <v>0.999533</v>
       </c>
       <c r="P16" t="n">
-        <v>0.998916</v>
+        <v>0.999637</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.00120149750311852</v>
+        <v>0.000297939591192581</v>
       </c>
       <c r="R16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S16" t="n">
-        <v>37.691082</v>
+        <v>42.319397</v>
       </c>
       <c r="T16" t="n">
-        <v>42.523937</v>
+        <v>63.427686</v>
       </c>
       <c r="U16" t="n">
-        <v>39.6199105</v>
+        <v>51.3871813333333</v>
       </c>
       <c r="V16" t="n">
-        <v>39.1323115</v>
+        <v>48.414461</v>
       </c>
       <c r="W16" t="n">
-        <v>2.05788132260188</v>
+        <v>10.8635981959036</v>
       </c>
       <c r="X16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y16" t="n">
         <v>0.014514</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.014514</v>
+        <v>0.09071</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.014514</v>
+        <v>0.054426</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.014514</v>
+        <v>0.058054</v>
       </c>
       <c r="AC16" t="n">
-        <v>0</v>
+        <v>0.0382273382803459</v>
       </c>
       <c r="AD16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.054824338711126</v>
+        <v>0.110854890515279</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.117049138897126</v>
+        <v>0.295241415728882</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.0926644399393155</v>
+        <v>0.210552372888711</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.099392141074505</v>
+        <v>0.225560812421973</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.0291908838453579</v>
+        <v>0.0931049816766228</v>
       </c>
       <c r="AJ16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK16" t="n">
-        <v>0.14819769555288</v>
+        <v>0.167572046576051</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.29568862053676</v>
+        <v>0.360588658778743</v>
       </c>
       <c r="AM16" t="n">
-        <v>0.206943759337235</v>
+        <v>0.293723799455144</v>
       </c>
       <c r="AN16" t="n">
-        <v>0.19194436062965</v>
+        <v>0.35301069301064</v>
       </c>
       <c r="AO16" t="n">
-        <v>0.0675243566603791</v>
+        <v>0.109316306913226</v>
       </c>
       <c r="AP16" t="n">
         <v>0</v>
@@ -2783,112 +2783,112 @@
         <v>56</v>
       </c>
       <c r="F17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
-        <v>0.000699</v>
+        <v>0.000651</v>
       </c>
       <c r="H17" t="n">
-        <v>0.004841</v>
+        <v>0.001134</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00201775</v>
+        <v>0.000856333333333333</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0012655</v>
+        <v>0.000784</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00191984606587785</v>
+        <v>0.000249492150845138</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
-        <v>0.999494</v>
+        <v>0.99683</v>
       </c>
       <c r="N17" t="n">
-        <v>0.999976</v>
+        <v>0.999683</v>
       </c>
       <c r="O17" t="n">
-        <v>0.9996775</v>
+        <v>0.998567666666667</v>
       </c>
       <c r="P17" t="n">
-        <v>0.99962</v>
+        <v>0.99919</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.000210227654381295</v>
+        <v>0.00152491846776585</v>
       </c>
       <c r="R17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S17" t="n">
-        <v>42.19568</v>
+        <v>46.283916</v>
       </c>
       <c r="T17" t="n">
-        <v>62.269491</v>
+        <v>60.965952</v>
       </c>
       <c r="U17" t="n">
-        <v>49.3684265</v>
+        <v>53.5339836666667</v>
       </c>
       <c r="V17" t="n">
-        <v>46.5042675</v>
+        <v>53.352083</v>
       </c>
       <c r="W17" t="n">
-        <v>8.86179778702096</v>
+        <v>7.3427080267245</v>
       </c>
       <c r="X17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y17" t="n">
         <v>0.014514</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.439034</v>
+        <v>26.215076</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.139693</v>
+        <v>8.762548</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.052612</v>
+        <v>0.058054</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.202767463409032</v>
+        <v>15.114348286512</v>
       </c>
       <c r="AD17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.071093552349034</v>
+        <v>0.116948768970177</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.333562223925119</v>
+        <v>0.485065971104527</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.201012083363562</v>
+        <v>0.289445697037057</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.199696278590048</v>
+        <v>0.266322351036466</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.145601333530129</v>
+        <v>0.185144768963378</v>
       </c>
       <c r="AJ17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.126669001800946</v>
+        <v>0.162814849369173</v>
       </c>
       <c r="AL17" t="n">
-        <v>0.540891963746698</v>
+        <v>0.62215353276742</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.305169929736412</v>
+        <v>0.384403241411423</v>
       </c>
       <c r="AN17" t="n">
-        <v>0.276559376699003</v>
+        <v>0.368241342097675</v>
       </c>
       <c r="AO17" t="n">
-        <v>0.207973328535079</v>
+        <v>0.230095440542788</v>
       </c>
       <c r="AP17" t="n">
         <v>0</v>
@@ -2923,109 +2923,109 @@
         <v>4</v>
       </c>
       <c r="G18" t="n">
-        <v>0.000823</v>
+        <v>0.000368</v>
       </c>
       <c r="H18" t="n">
-        <v>0.001423</v>
+        <v>0.002139</v>
       </c>
       <c r="I18" t="n">
-        <v>0.001077</v>
+        <v>0.001114</v>
       </c>
       <c r="J18" t="n">
-        <v>0.001031</v>
+        <v>0.0009745</v>
       </c>
       <c r="K18" t="n">
-        <v>0.000252760756447673</v>
+        <v>0.000742489955038675</v>
       </c>
       <c r="L18" t="n">
         <v>4</v>
       </c>
       <c r="M18" t="n">
-        <v>0.99905</v>
+        <v>0.999409</v>
       </c>
       <c r="N18" t="n">
-        <v>0.999975</v>
+        <v>0.999995</v>
       </c>
       <c r="O18" t="n">
-        <v>0.99961925</v>
+        <v>0.999724</v>
       </c>
       <c r="P18" t="n">
-        <v>0.999726</v>
+        <v>0.999746</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.000442582101611276</v>
+        <v>0.000305699198559615</v>
       </c>
       <c r="R18" t="n">
         <v>4</v>
       </c>
       <c r="S18" t="n">
-        <v>38.036717</v>
+        <v>42.111092</v>
       </c>
       <c r="T18" t="n">
-        <v>64.33913</v>
+        <v>62.234621</v>
       </c>
       <c r="U18" t="n">
-        <v>47.012045</v>
+        <v>50.58734125</v>
       </c>
       <c r="V18" t="n">
-        <v>42.8361665</v>
+        <v>49.001826</v>
       </c>
       <c r="W18" t="n">
-        <v>11.7979477838089</v>
+        <v>8.92180720782097</v>
       </c>
       <c r="X18" t="n">
         <v>4</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.439034</v>
+        <v>0.711163</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.17053375</v>
+        <v>0.338347</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.105223</v>
+        <v>0.3138555</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.19162998315395</v>
+        <v>0.376062900826444</v>
       </c>
       <c r="AD18" t="n">
         <v>4</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.0939397452294676</v>
+        <v>0.0788229058864805</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.438126459948937</v>
+        <v>0.463805863837215</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.237826114738521</v>
+        <v>0.204139132457792</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.209619126887839</v>
+        <v>0.136963880053736</v>
       </c>
       <c r="AI18" t="n">
-        <v>0.168054714007132</v>
+        <v>0.179217526328107</v>
       </c>
       <c r="AJ18" t="n">
         <v>4</v>
       </c>
       <c r="AK18" t="n">
-        <v>0.125723356620159</v>
+        <v>0.111926610491855</v>
       </c>
       <c r="AL18" t="n">
-        <v>0.578898706408148</v>
+        <v>0.91846164707884</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.325165388789682</v>
+        <v>0.391634695416922</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.298019746065211</v>
+        <v>0.268075262048496</v>
       </c>
       <c r="AO18" t="n">
-        <v>0.222836381969387</v>
+        <v>0.374246822710395</v>
       </c>
       <c r="AP18" t="n">
         <v>0</v>
@@ -3060,109 +3060,109 @@
         <v>4</v>
       </c>
       <c r="G19" t="n">
-        <v>0.000465</v>
+        <v>0.00062</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001913</v>
+        <v>0.001998</v>
       </c>
       <c r="I19" t="n">
-        <v>0.00109675</v>
+        <v>0.00132175</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0010045</v>
+        <v>0.0013345</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0006374837906436</v>
+        <v>0.000675451639028781</v>
       </c>
       <c r="L19" t="n">
         <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>0.999008</v>
+        <v>0.999181</v>
       </c>
       <c r="N19" t="n">
-        <v>0.99999</v>
+        <v>0.999991</v>
       </c>
       <c r="O19" t="n">
-        <v>0.999486</v>
+        <v>0.9996455</v>
       </c>
       <c r="P19" t="n">
-        <v>0.999473</v>
+        <v>0.999705</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.000545666564854401</v>
+        <v>0.000393793092879988</v>
       </c>
       <c r="R19" t="n">
         <v>4</v>
       </c>
       <c r="S19" t="n">
-        <v>34.42806</v>
+        <v>23.142818</v>
       </c>
       <c r="T19" t="n">
-        <v>62.819747</v>
+        <v>56.63966</v>
       </c>
       <c r="U19" t="n">
-        <v>47.702706</v>
+        <v>44.34371225</v>
       </c>
       <c r="V19" t="n">
-        <v>46.7815085</v>
+        <v>48.7961855</v>
       </c>
       <c r="W19" t="n">
-        <v>11.6586527749944</v>
+        <v>14.8594729893869</v>
       </c>
       <c r="X19" t="n">
         <v>4</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.014514</v>
+        <v>0.032655</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.232217</v>
+        <v>0.522487</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.1233655</v>
+        <v>0.2630575</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.1233655</v>
+        <v>0.248544</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.125690885653389</v>
+        <v>0.253891801785065</v>
       </c>
       <c r="AD19" t="n">
         <v>4</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.0780663217873339</v>
+        <v>0.064123526597</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.427487314222482</v>
+        <v>0.559375101445209</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.212941995930709</v>
+        <v>0.233904705791873</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.17310717385651</v>
+        <v>0.156060097562642</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.163611190317775</v>
+        <v>0.227785668578554</v>
       </c>
       <c r="AJ19" t="n">
         <v>4</v>
       </c>
       <c r="AK19" t="n">
-        <v>0.109857763379781</v>
+        <v>0.181529754401931</v>
       </c>
       <c r="AL19" t="n">
-        <v>0.62889135193001</v>
+        <v>0.679911195549716</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.321362393103858</v>
+        <v>0.352358078713472</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.27335022855282</v>
+        <v>0.27399568245112</v>
       </c>
       <c r="AO19" t="n">
-        <v>0.243896608063934</v>
+        <v>0.234848349138564</v>
       </c>
       <c r="AP19" t="n">
         <v>0</v>
@@ -3194,112 +3194,112 @@
         <v>55</v>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20" t="n">
-        <v>0.000149</v>
+        <v>0.000823</v>
       </c>
       <c r="H20" t="n">
-        <v>0.000899</v>
+        <v>0.001423</v>
       </c>
       <c r="I20" t="n">
-        <v>0.000574666666666667</v>
+        <v>0.001077</v>
       </c>
       <c r="J20" t="n">
-        <v>0.000676</v>
+        <v>0.001031</v>
       </c>
       <c r="K20" t="n">
-        <v>0.000385131579247059</v>
+        <v>0.000252760756447673</v>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
-        <v>0.999197</v>
+        <v>0.99905</v>
       </c>
       <c r="N20" t="n">
-        <v>0.999765</v>
+        <v>0.999975</v>
       </c>
       <c r="O20" t="n">
-        <v>0.999533</v>
+        <v>0.99961925</v>
       </c>
       <c r="P20" t="n">
-        <v>0.999637</v>
+        <v>0.999726</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.000297939591192581</v>
+        <v>0.000442582101611276</v>
       </c>
       <c r="R20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S20" t="n">
-        <v>42.319397</v>
+        <v>38.036717</v>
       </c>
       <c r="T20" t="n">
-        <v>63.427686</v>
+        <v>64.33913</v>
       </c>
       <c r="U20" t="n">
-        <v>51.3871813333333</v>
+        <v>47.012045</v>
       </c>
       <c r="V20" t="n">
-        <v>48.414461</v>
+        <v>42.8361665</v>
       </c>
       <c r="W20" t="n">
-        <v>10.8635981959036</v>
+        <v>11.7979477838089</v>
       </c>
       <c r="X20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.014514</v>
+        <v>0.032655</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.09071</v>
+        <v>0.439034</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.054426</v>
+        <v>0.17053375</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.058054</v>
+        <v>0.105223</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.0382273382803459</v>
+        <v>0.19162998315395</v>
       </c>
       <c r="AD20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.110854890515279</v>
+        <v>0.0939397452294676</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.295241415728882</v>
+        <v>0.438126459948937</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.210552372888711</v>
+        <v>0.237826114738521</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.225560812421973</v>
+        <v>0.209619126887839</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.0931049816766228</v>
+        <v>0.168054714007132</v>
       </c>
       <c r="AJ20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK20" t="n">
-        <v>0.167572046576051</v>
+        <v>0.125723356620159</v>
       </c>
       <c r="AL20" t="n">
-        <v>0.360588658778743</v>
+        <v>0.578898706408148</v>
       </c>
       <c r="AM20" t="n">
-        <v>0.293723799455144</v>
+        <v>0.325165388789682</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.35301069301064</v>
+        <v>0.298019746065211</v>
       </c>
       <c r="AO20" t="n">
-        <v>0.109316306913226</v>
+        <v>0.222836381969387</v>
       </c>
       <c r="AP20" t="n">
         <v>0</v>
@@ -3331,112 +3331,112 @@
         <v>56</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" t="n">
-        <v>0.000651</v>
+        <v>0.000465</v>
       </c>
       <c r="H21" t="n">
-        <v>0.001134</v>
+        <v>0.001913</v>
       </c>
       <c r="I21" t="n">
-        <v>0.000856333333333333</v>
+        <v>0.00109675</v>
       </c>
       <c r="J21" t="n">
-        <v>0.000784</v>
+        <v>0.0010045</v>
       </c>
       <c r="K21" t="n">
-        <v>0.000249492150845138</v>
+        <v>0.0006374837906436</v>
       </c>
       <c r="L21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M21" t="n">
-        <v>0.99683</v>
+        <v>0.999008</v>
       </c>
       <c r="N21" t="n">
-        <v>0.999683</v>
+        <v>0.99999</v>
       </c>
       <c r="O21" t="n">
-        <v>0.998567666666667</v>
+        <v>0.999486</v>
       </c>
       <c r="P21" t="n">
-        <v>0.99919</v>
+        <v>0.999473</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.00152491846776585</v>
+        <v>0.000545666564854401</v>
       </c>
       <c r="R21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S21" t="n">
-        <v>46.283916</v>
+        <v>34.42806</v>
       </c>
       <c r="T21" t="n">
-        <v>60.965952</v>
+        <v>62.819747</v>
       </c>
       <c r="U21" t="n">
-        <v>53.5339836666667</v>
+        <v>47.702706</v>
       </c>
       <c r="V21" t="n">
-        <v>53.352083</v>
+        <v>46.7815085</v>
       </c>
       <c r="W21" t="n">
-        <v>7.3427080267245</v>
+        <v>11.6586527749944</v>
       </c>
       <c r="X21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y21" t="n">
         <v>0.014514</v>
       </c>
       <c r="Z21" t="n">
-        <v>26.215076</v>
+        <v>0.232217</v>
       </c>
       <c r="AA21" t="n">
-        <v>8.762548</v>
+        <v>0.1233655</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.058054</v>
+        <v>0.1233655</v>
       </c>
       <c r="AC21" t="n">
-        <v>15.114348286512</v>
+        <v>0.125690885653389</v>
       </c>
       <c r="AD21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.116948768970177</v>
+        <v>0.0780663217873339</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.485065971104527</v>
+        <v>0.427487314222482</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.289445697037057</v>
+        <v>0.212941995930709</v>
       </c>
       <c r="AH21" t="n">
-        <v>0.266322351036466</v>
+        <v>0.17310717385651</v>
       </c>
       <c r="AI21" t="n">
-        <v>0.185144768963378</v>
+        <v>0.163611190317775</v>
       </c>
       <c r="AJ21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK21" t="n">
-        <v>0.162814849369173</v>
+        <v>0.109857763379781</v>
       </c>
       <c r="AL21" t="n">
-        <v>0.62215353276742</v>
+        <v>0.62889135193001</v>
       </c>
       <c r="AM21" t="n">
-        <v>0.384403241411423</v>
+        <v>0.321362393103858</v>
       </c>
       <c r="AN21" t="n">
-        <v>0.368241342097675</v>
+        <v>0.27335022855282</v>
       </c>
       <c r="AO21" t="n">
-        <v>0.230095440542788</v>
+        <v>0.243896608063934</v>
       </c>
       <c r="AP21" t="n">
         <v>0</v>
@@ -3471,55 +3471,55 @@
         <v>4</v>
       </c>
       <c r="G22" t="n">
-        <v>0.000368</v>
+        <v>0.00133</v>
       </c>
       <c r="H22" t="n">
-        <v>0.002139</v>
+        <v>0.002509</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001114</v>
+        <v>0.0016735</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0009745</v>
+        <v>0.0014275</v>
       </c>
       <c r="K22" t="n">
-        <v>0.000742489955038675</v>
+        <v>0.000562193620265</v>
       </c>
       <c r="L22" t="n">
         <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>0.999409</v>
+        <v>0.996841</v>
       </c>
       <c r="N22" t="n">
-        <v>0.999995</v>
+        <v>0.99946</v>
       </c>
       <c r="O22" t="n">
-        <v>0.999724</v>
+        <v>0.99853325</v>
       </c>
       <c r="P22" t="n">
-        <v>0.999746</v>
+        <v>0.998916</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.000305699198559615</v>
+        <v>0.00120149750311852</v>
       </c>
       <c r="R22" t="n">
         <v>4</v>
       </c>
       <c r="S22" t="n">
-        <v>42.111092</v>
+        <v>37.691082</v>
       </c>
       <c r="T22" t="n">
-        <v>62.234621</v>
+        <v>42.523937</v>
       </c>
       <c r="U22" t="n">
-        <v>50.58734125</v>
+        <v>39.6199105</v>
       </c>
       <c r="V22" t="n">
-        <v>49.001826</v>
+        <v>39.1323115</v>
       </c>
       <c r="W22" t="n">
-        <v>8.92180720782097</v>
+        <v>2.05788132260188</v>
       </c>
       <c r="X22" t="n">
         <v>4</v>
@@ -3528,52 +3528,52 @@
         <v>0.014514</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.711163</v>
+        <v>0.014514</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.338347</v>
+        <v>0.014514</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.3138555</v>
+        <v>0.014514</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.376062900826444</v>
+        <v>0</v>
       </c>
       <c r="AD22" t="n">
         <v>4</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.0788229058864805</v>
+        <v>0.054824338711126</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.463805863837215</v>
+        <v>0.117049138897126</v>
       </c>
       <c r="AG22" t="n">
-        <v>0.204139132457792</v>
+        <v>0.0926644399393155</v>
       </c>
       <c r="AH22" t="n">
-        <v>0.136963880053736</v>
+        <v>0.099392141074505</v>
       </c>
       <c r="AI22" t="n">
-        <v>0.179217526328107</v>
+        <v>0.0291908838453579</v>
       </c>
       <c r="AJ22" t="n">
         <v>4</v>
       </c>
       <c r="AK22" t="n">
-        <v>0.111926610491855</v>
+        <v>0.14819769555288</v>
       </c>
       <c r="AL22" t="n">
-        <v>0.91846164707884</v>
+        <v>0.29568862053676</v>
       </c>
       <c r="AM22" t="n">
-        <v>0.391634695416922</v>
+        <v>0.206943759337235</v>
       </c>
       <c r="AN22" t="n">
-        <v>0.268075262048496</v>
+        <v>0.19194436062965</v>
       </c>
       <c r="AO22" t="n">
-        <v>0.374246822710395</v>
+        <v>0.0675243566603791</v>
       </c>
       <c r="AP22" t="n">
         <v>0</v>
@@ -3608,109 +3608,109 @@
         <v>4</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00062</v>
+        <v>0.000699</v>
       </c>
       <c r="H23" t="n">
-        <v>0.001998</v>
+        <v>0.004841</v>
       </c>
       <c r="I23" t="n">
-        <v>0.00132175</v>
+        <v>0.00201775</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0013345</v>
+        <v>0.0012655</v>
       </c>
       <c r="K23" t="n">
-        <v>0.000675451639028781</v>
+        <v>0.00191984606587785</v>
       </c>
       <c r="L23" t="n">
         <v>4</v>
       </c>
       <c r="M23" t="n">
-        <v>0.999181</v>
+        <v>0.999494</v>
       </c>
       <c r="N23" t="n">
-        <v>0.999991</v>
+        <v>0.999976</v>
       </c>
       <c r="O23" t="n">
-        <v>0.9996455</v>
+        <v>0.9996775</v>
       </c>
       <c r="P23" t="n">
-        <v>0.999705</v>
+        <v>0.99962</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.000393793092879988</v>
+        <v>0.000210227654381295</v>
       </c>
       <c r="R23" t="n">
         <v>4</v>
       </c>
       <c r="S23" t="n">
-        <v>23.142818</v>
+        <v>42.19568</v>
       </c>
       <c r="T23" t="n">
-        <v>56.63966</v>
+        <v>62.269491</v>
       </c>
       <c r="U23" t="n">
-        <v>44.34371225</v>
+        <v>49.3684265</v>
       </c>
       <c r="V23" t="n">
-        <v>48.7961855</v>
+        <v>46.5042675</v>
       </c>
       <c r="W23" t="n">
-        <v>14.8594729893869</v>
+        <v>8.86179778702096</v>
       </c>
       <c r="X23" t="n">
         <v>4</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.522487</v>
+        <v>0.439034</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.2630575</v>
+        <v>0.139693</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.248544</v>
+        <v>0.052612</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.253891801785065</v>
+        <v>0.202767463409032</v>
       </c>
       <c r="AD23" t="n">
         <v>4</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.064123526597</v>
+        <v>0.071093552349034</v>
       </c>
       <c r="AF23" t="n">
-        <v>0.559375101445209</v>
+        <v>0.333562223925119</v>
       </c>
       <c r="AG23" t="n">
-        <v>0.233904705791873</v>
+        <v>0.201012083363562</v>
       </c>
       <c r="AH23" t="n">
-        <v>0.156060097562642</v>
+        <v>0.199696278590048</v>
       </c>
       <c r="AI23" t="n">
-        <v>0.227785668578554</v>
+        <v>0.145601333530129</v>
       </c>
       <c r="AJ23" t="n">
         <v>4</v>
       </c>
       <c r="AK23" t="n">
-        <v>0.181529754401931</v>
+        <v>0.126669001800946</v>
       </c>
       <c r="AL23" t="n">
-        <v>0.679911195549716</v>
+        <v>0.540891963746698</v>
       </c>
       <c r="AM23" t="n">
-        <v>0.352358078713472</v>
+        <v>0.305169929736412</v>
       </c>
       <c r="AN23" t="n">
-        <v>0.27399568245112</v>
+        <v>0.276559376699003</v>
       </c>
       <c r="AO23" t="n">
-        <v>0.234848349138564</v>
+        <v>0.207973328535079</v>
       </c>
       <c r="AP23" t="n">
         <v>0</v>
@@ -3743,127 +3743,127 @@
         <v>10</v>
       </c>
       <c r="G24" t="n">
-        <v>0.000398862</v>
+        <v>0.0003988616117</v>
       </c>
       <c r="H24" t="n">
-        <v>0.00624885</v>
+        <v>0.006248850204</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0025091702</v>
+        <v>0.00250917018317</v>
       </c>
       <c r="J24" t="n">
-        <v>0.002527304</v>
+        <v>0.0025273042215</v>
       </c>
       <c r="K24" t="n">
-        <v>0.00159406213840963</v>
+        <v>0.0015940623180431</v>
       </c>
       <c r="L24" t="n">
         <v>10</v>
       </c>
       <c r="M24" t="n">
-        <v>0.996792344</v>
+        <v>0.9971469768</v>
       </c>
       <c r="N24" t="n">
-        <v>0.998939031</v>
+        <v>0.9992552423</v>
       </c>
       <c r="O24" t="n">
-        <v>0.9982899697</v>
+        <v>0.9986918351</v>
       </c>
       <c r="P24" t="n">
-        <v>0.9983774035</v>
+        <v>0.99897217905</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.000660412964734438</v>
+        <v>0.000669120991224029</v>
       </c>
       <c r="R24" t="n">
         <v>10</v>
       </c>
       <c r="S24" t="n">
-        <v>1.607141904</v>
+        <v>1.769674314</v>
       </c>
       <c r="T24" t="n">
-        <v>9.356764506</v>
+        <v>12.03945469</v>
       </c>
       <c r="U24" t="n">
-        <v>5.1238093155</v>
+        <v>6.0620607153</v>
       </c>
       <c r="V24" t="n">
-        <v>4.212504274</v>
+        <v>4.748517298</v>
       </c>
       <c r="W24" t="n">
-        <v>3.18298695174698</v>
+        <v>4.09498354707606</v>
       </c>
       <c r="X24" t="n">
         <v>10</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.248357109</v>
+        <v>0.2005966173</v>
       </c>
       <c r="Z24" t="n">
-        <v>24.15583065</v>
+        <v>13.18123281</v>
       </c>
       <c r="AA24" t="n">
-        <v>8.7661719307</v>
+        <v>3.50553506317</v>
       </c>
       <c r="AB24" t="n">
-        <v>4.433440772</v>
+        <v>2.0870906735</v>
       </c>
       <c r="AC24" t="n">
-        <v>9.11923963105113</v>
+        <v>4.18061208068768</v>
       </c>
       <c r="AD24" t="n">
         <v>10</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.235830962</v>
+        <v>0.2441171874</v>
       </c>
       <c r="AF24" t="n">
-        <v>1.575018208</v>
+        <v>1.594739528</v>
       </c>
       <c r="AG24" t="n">
-        <v>0.6374410919</v>
+        <v>0.67285357242</v>
       </c>
       <c r="AH24" t="n">
-        <v>0.501941786</v>
+        <v>0.5284645173</v>
       </c>
       <c r="AI24" t="n">
-        <v>0.462237506254664</v>
+        <v>0.465620066252572</v>
       </c>
       <c r="AJ24" t="n">
         <v>10</v>
       </c>
       <c r="AK24" t="n">
-        <v>0.725775631</v>
+        <v>0.7705203453</v>
       </c>
       <c r="AL24" t="n">
-        <v>2.830659827</v>
+        <v>2.713974409</v>
       </c>
       <c r="AM24" t="n">
-        <v>1.4110001238</v>
+        <v>1.48660996946</v>
       </c>
       <c r="AN24" t="n">
-        <v>1.325131796</v>
+        <v>1.4050049855</v>
       </c>
       <c r="AO24" t="n">
-        <v>0.704887858336971</v>
+        <v>0.702315616316955</v>
       </c>
       <c r="AP24" t="n">
         <v>10</v>
       </c>
       <c r="AQ24" t="n">
-        <v>0.017151313</v>
+        <v>0.01715131292</v>
       </c>
       <c r="AR24" t="n">
         <v>0.020194359</v>
       </c>
       <c r="AS24" t="n">
-        <v>0.0182728539</v>
+        <v>0.018272853897</v>
       </c>
       <c r="AT24" t="n">
-        <v>0.0182266815</v>
+        <v>0.01822668166</v>
       </c>
       <c r="AU24" t="n">
-        <v>0.000878257693125864</v>
+        <v>0.000878257672528257</v>
       </c>
     </row>
     <row r="25">
@@ -3882,127 +3882,127 @@
         <v>10</v>
       </c>
       <c r="G25" t="n">
-        <v>0.001314596</v>
+        <v>0.001314585174</v>
       </c>
       <c r="H25" t="n">
-        <v>0.008242305</v>
+        <v>0.008242304939</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0030219988</v>
+        <v>0.0030219976132</v>
       </c>
       <c r="J25" t="n">
-        <v>0.00208987</v>
+        <v>0.0020898700445</v>
       </c>
       <c r="K25" t="n">
-        <v>0.00221286552934715</v>
+        <v>0.00221286638474041</v>
       </c>
       <c r="L25" t="n">
         <v>10</v>
       </c>
       <c r="M25" t="n">
-        <v>0.997168268</v>
+        <v>0.9972427458</v>
       </c>
       <c r="N25" t="n">
-        <v>0.999362922</v>
+        <v>0.9992220177</v>
       </c>
       <c r="O25" t="n">
-        <v>0.9986346165</v>
+        <v>0.99826559723</v>
       </c>
       <c r="P25" t="n">
-        <v>0.9987534605</v>
+        <v>0.99836592175</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.000608476303945303</v>
+        <v>0.000635863202676508</v>
       </c>
       <c r="R25" t="n">
         <v>10</v>
       </c>
       <c r="S25" t="n">
-        <v>1.993351348</v>
+        <v>2.255922934</v>
       </c>
       <c r="T25" t="n">
-        <v>5.349714799</v>
+        <v>6.294519503</v>
       </c>
       <c r="U25" t="n">
-        <v>3.3274999346</v>
+        <v>3.8962633017</v>
       </c>
       <c r="V25" t="n">
-        <v>3.000694141</v>
+        <v>3.524736661</v>
       </c>
       <c r="W25" t="n">
-        <v>1.11800867488601</v>
+        <v>1.41058586976318</v>
       </c>
       <c r="X25" t="n">
         <v>10</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.41715515</v>
+        <v>0.2848187271</v>
       </c>
       <c r="Z25" t="n">
-        <v>4.114056954</v>
+        <v>3.762199924</v>
       </c>
       <c r="AA25" t="n">
-        <v>1.8025340281</v>
+        <v>0.92900330236</v>
       </c>
       <c r="AB25" t="n">
-        <v>1.6359525285</v>
+        <v>0.59281379705</v>
       </c>
       <c r="AC25" t="n">
-        <v>1.17563082133011</v>
+        <v>1.05184354810093</v>
       </c>
       <c r="AD25" t="n">
         <v>10</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.219242261</v>
+        <v>0.2533298612</v>
       </c>
       <c r="AF25" t="n">
-        <v>0.522489478</v>
+        <v>0.5831522012</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.4015471314</v>
+        <v>0.46613344764</v>
       </c>
       <c r="AH25" t="n">
-        <v>0.4255345725</v>
+        <v>0.4944262318</v>
       </c>
       <c r="AI25" t="n">
-        <v>0.0981869873423096</v>
+        <v>0.112030887027972</v>
       </c>
       <c r="AJ25" t="n">
         <v>10</v>
       </c>
       <c r="AK25" t="n">
-        <v>0.658570814</v>
+        <v>0.6931811469</v>
       </c>
       <c r="AL25" t="n">
-        <v>1.603440466</v>
+        <v>2.067776774</v>
       </c>
       <c r="AM25" t="n">
-        <v>0.9324720787</v>
+        <v>1.10154727655</v>
       </c>
       <c r="AN25" t="n">
-        <v>0.8937336505</v>
+        <v>1.052796587</v>
       </c>
       <c r="AO25" t="n">
-        <v>0.264514936071645</v>
+        <v>0.375727820164045</v>
       </c>
       <c r="AP25" t="n">
         <v>10</v>
       </c>
       <c r="AQ25" t="n">
-        <v>0.01613179</v>
+        <v>0.01613178951</v>
       </c>
       <c r="AR25" t="n">
-        <v>0.018762949</v>
+        <v>0.01876294872</v>
       </c>
       <c r="AS25" t="n">
-        <v>0.0177476984</v>
+        <v>0.017747698141</v>
       </c>
       <c r="AT25" t="n">
-        <v>0.0177524875</v>
+        <v>0.017752487855</v>
       </c>
       <c r="AU25" t="n">
-        <v>0.00071299859445883</v>
+        <v>0.000712998570275664</v>
       </c>
     </row>
     <row r="26">
@@ -4021,127 +4021,127 @@
         <v>10</v>
       </c>
       <c r="G26" t="n">
-        <v>0.001145127</v>
+        <v>0.001145127179</v>
       </c>
       <c r="H26" t="n">
-        <v>0.007925134</v>
+        <v>0.007925134399</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0039495033</v>
+        <v>0.0039495032771</v>
       </c>
       <c r="J26" t="n">
-        <v>0.003948191</v>
+        <v>0.003948190654</v>
       </c>
       <c r="K26" t="n">
-        <v>0.00240759811464511</v>
+        <v>0.00240759816379076</v>
       </c>
       <c r="L26" t="n">
         <v>10</v>
       </c>
       <c r="M26" t="n">
-        <v>0.996254709</v>
+        <v>0.9928499718</v>
       </c>
       <c r="N26" t="n">
-        <v>0.99936771</v>
+        <v>0.9993623986</v>
       </c>
       <c r="O26" t="n">
-        <v>0.9981114201</v>
+        <v>0.99769002696</v>
       </c>
       <c r="P26" t="n">
-        <v>0.998481918</v>
+        <v>0.99817542905</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.00110214486969166</v>
+        <v>0.00183711699581496</v>
       </c>
       <c r="R26" t="n">
         <v>10</v>
       </c>
       <c r="S26" t="n">
-        <v>0.792990213</v>
+        <v>0.7917519407</v>
       </c>
       <c r="T26" t="n">
-        <v>5.645974739</v>
+        <v>7.543740545</v>
       </c>
       <c r="U26" t="n">
-        <v>2.4844424275</v>
+        <v>2.94539355805</v>
       </c>
       <c r="V26" t="n">
-        <v>2.331420808</v>
+        <v>2.6689953435</v>
       </c>
       <c r="W26" t="n">
-        <v>1.56413180311925</v>
+        <v>2.12485752217538</v>
       </c>
       <c r="X26" t="n">
         <v>10</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.184851107</v>
+        <v>0.02152383454</v>
       </c>
       <c r="Z26" t="n">
-        <v>577.7743903</v>
+        <v>30.44265429</v>
       </c>
       <c r="AA26" t="n">
-        <v>61.7032889606</v>
+        <v>3.95690106377</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.7104902585</v>
+        <v>0.30782186185</v>
       </c>
       <c r="AC26" t="n">
-        <v>181.562459386594</v>
+        <v>9.49128199721987</v>
       </c>
       <c r="AD26" t="n">
         <v>10</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.19885573</v>
+        <v>0.2084701882</v>
       </c>
       <c r="AF26" t="n">
-        <v>0.541497278</v>
+        <v>1.150174306</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.3823504885</v>
+        <v>0.50158616066</v>
       </c>
       <c r="AH26" t="n">
-        <v>0.4092874525</v>
+        <v>0.42272365055</v>
       </c>
       <c r="AI26" t="n">
-        <v>0.124197854735376</v>
+        <v>0.299034695807762</v>
       </c>
       <c r="AJ26" t="n">
         <v>10</v>
       </c>
       <c r="AK26" t="n">
-        <v>0.419978432</v>
+        <v>0.57369698</v>
       </c>
       <c r="AL26" t="n">
-        <v>1.225121517</v>
+        <v>1.787192949</v>
       </c>
       <c r="AM26" t="n">
-        <v>0.797773095</v>
+        <v>1.01584380479</v>
       </c>
       <c r="AN26" t="n">
-        <v>0.7660797075</v>
+        <v>1.01784635075</v>
       </c>
       <c r="AO26" t="n">
-        <v>0.270150181806484</v>
+        <v>0.403063682938889</v>
       </c>
       <c r="AP26" t="n">
         <v>10</v>
       </c>
       <c r="AQ26" t="n">
-        <v>0.016852209</v>
+        <v>0.01685220944</v>
       </c>
       <c r="AR26" t="n">
-        <v>0.020010196</v>
+        <v>0.02001019556</v>
       </c>
       <c r="AS26" t="n">
-        <v>0.0182826541</v>
+        <v>0.018282654111</v>
       </c>
       <c r="AT26" t="n">
-        <v>0.018021192</v>
+        <v>0.01802119204</v>
       </c>
       <c r="AU26" t="n">
-        <v>0.00107676797229636</v>
+        <v>0.00107676785144076</v>
       </c>
     </row>
     <row r="27">
@@ -4160,127 +4160,127 @@
         <v>10</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00033554</v>
+        <v>0.0003355399204</v>
       </c>
       <c r="H27" t="n">
-        <v>0.007887921</v>
+        <v>0.007887921169</v>
       </c>
       <c r="I27" t="n">
-        <v>0.004067979</v>
+        <v>0.00406797889164</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0041151625</v>
+        <v>0.004115162413</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0024718229660545</v>
+        <v>0.00247182300139559</v>
       </c>
       <c r="L27" t="n">
         <v>10</v>
       </c>
       <c r="M27" t="n">
-        <v>0.995283554</v>
+        <v>0.9966382578</v>
       </c>
       <c r="N27" t="n">
-        <v>0.999283158</v>
+        <v>0.9993224798</v>
       </c>
       <c r="O27" t="n">
-        <v>0.9981253555</v>
+        <v>0.99806163233</v>
       </c>
       <c r="P27" t="n">
-        <v>0.99870663</v>
+        <v>0.99805653705</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.0012222092341113</v>
+        <v>0.000979921925394358</v>
       </c>
       <c r="R27" t="n">
         <v>10</v>
       </c>
       <c r="S27" t="n">
-        <v>0.80637089</v>
+        <v>0.8045920272</v>
       </c>
       <c r="T27" t="n">
-        <v>6.43937731</v>
+        <v>8.282732173</v>
       </c>
       <c r="U27" t="n">
-        <v>2.015845322</v>
+        <v>2.28193160212</v>
       </c>
       <c r="V27" t="n">
-        <v>1.50246833</v>
+        <v>1.6048065225</v>
       </c>
       <c r="W27" t="n">
-        <v>1.67551755443517</v>
+        <v>2.22253004485359</v>
       </c>
       <c r="X27" t="n">
         <v>10</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.214647035</v>
+        <v>0.02156230635</v>
       </c>
       <c r="Z27" t="n">
-        <v>20.87710489</v>
+        <v>4.325433284</v>
       </c>
       <c r="AA27" t="n">
-        <v>3.0847990124</v>
+        <v>1.282316682285</v>
       </c>
       <c r="AB27" t="n">
-        <v>1.2015866135</v>
+        <v>0.8927567086</v>
       </c>
       <c r="AC27" t="n">
-        <v>6.31060208252266</v>
+        <v>1.35045964651512</v>
       </c>
       <c r="AD27" t="n">
         <v>10</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.150247611</v>
+        <v>0.1553091062</v>
       </c>
       <c r="AF27" t="n">
-        <v>0.914044976</v>
+        <v>1.190505461</v>
       </c>
       <c r="AG27" t="n">
-        <v>0.4421032418</v>
+        <v>0.4755975402</v>
       </c>
       <c r="AH27" t="n">
-        <v>0.3462053065</v>
+        <v>0.38338017255</v>
       </c>
       <c r="AI27" t="n">
-        <v>0.287507408089891</v>
+        <v>0.33094944141215</v>
       </c>
       <c r="AJ27" t="n">
         <v>10</v>
       </c>
       <c r="AK27" t="n">
-        <v>0.362871045</v>
+        <v>0.362854394</v>
       </c>
       <c r="AL27" t="n">
-        <v>1.61062611</v>
+        <v>1.642895783</v>
       </c>
       <c r="AM27" t="n">
-        <v>0.7489928735</v>
+        <v>0.8264280048</v>
       </c>
       <c r="AN27" t="n">
-        <v>0.5826802045</v>
+        <v>0.7000490524</v>
       </c>
       <c r="AO27" t="n">
-        <v>0.413819996394498</v>
+        <v>0.458097516235459</v>
       </c>
       <c r="AP27" t="n">
         <v>10</v>
       </c>
       <c r="AQ27" t="n">
-        <v>0.016852429</v>
+        <v>0.01685242918</v>
       </c>
       <c r="AR27" t="n">
-        <v>0.018977718</v>
+        <v>0.01897771794</v>
       </c>
       <c r="AS27" t="n">
-        <v>0.0177845691</v>
+        <v>0.017784568971</v>
       </c>
       <c r="AT27" t="n">
-        <v>0.0176547105</v>
+        <v>0.0176547103</v>
       </c>
       <c r="AU27" t="n">
-        <v>0.000746777816453901</v>
+        <v>0.000746777761139035</v>
       </c>
     </row>
     <row r="28">

</xml_diff>